<commit_message>
update n exit q exit()
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lethihongnhung/Desktop/PP-so/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27164237-5A9F-9C4A-8619-5F23B392DFB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1CAEA2-DA38-6F41-9ED6-9DB72F3DB6AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{9746C11F-56AA-B54F-ADE6-2290D58A1BDE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9746C11F-56AA-B54F-ADE6-2290D58A1BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ECBCCA9-DFEE-9D4B-A2A5-309CDD69CAFB}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -408,34 +408,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>2.4500000000000002</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1.7</v>
+        <v>0.2</v>
       </c>
       <c r="B3">
-        <v>3.35</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1.5</v>
+        <v>0.4</v>
       </c>
       <c r="B4">
-        <v>3.87</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1.6</v>
+        <v>0.6</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.8</v>
+      </c>
+      <c r="B6">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1.2</v>
+      </c>
+      <c r="B8">
+        <v>1.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>